<commit_message>
v2.1.1 HTML files fixed
</commit_message>
<xml_diff>
--- a/v2.1.1/dist/cl/xlsx/ESPD-CriteriaTaxonomy-BASIC-V2.1.1.xlsx
+++ b/v2.1.1/dist/cl/xlsx/ESPD-CriteriaTaxonomy-BASIC-V2.1.1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\ESPD\GitHub\ESPD-EDM\docs\src\main\asciidoc\dist\cl\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrevenga\Documents\git\ESPD-EDM\ESPD-EDM\docs\src\main\asciidoc\dist\cl\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="588" firstSheet="31" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11408" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11440" uniqueCount="452">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2466,49 +2466,49 @@
     <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hipervínculo" xfId="42"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4343,7 +4343,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4632,9 +4632,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:Z146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="55" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="10.7109375" style="25" customWidth="1"/>
@@ -12151,7 +12151,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="2" customWidth="1"/>
@@ -13566,7 +13566,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -15539,7 +15539,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="68" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="66" bestFit="1" customWidth="1"/>
@@ -16369,7 +16369,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -17219,7 +17219,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="7" customWidth="1"/>
@@ -18052,7 +18052,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -18900,7 +18900,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="57" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="54" bestFit="1" customWidth="1"/>
@@ -19824,7 +19824,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="80" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="15" customWidth="1"/>
@@ -20744,7 +20744,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="57" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="54" customWidth="1"/>
@@ -21661,7 +21661,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="57" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="54" customWidth="1"/>
@@ -22569,7 +22569,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="10.7109375" style="15" customWidth="1"/>
@@ -26061,7 +26061,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" style="25" customWidth="1"/>
@@ -28494,7 +28494,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" style="10" customWidth="1"/>
@@ -33392,7 +33392,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="10" customWidth="1"/>
@@ -34184,7 +34184,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="10" customWidth="1"/>
@@ -36403,7 +36403,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -37306,7 +37306,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="10" customWidth="1"/>
@@ -38708,7 +38708,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -41309,7 +41309,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
@@ -42895,7 +42895,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="38" customWidth="1"/>
@@ -45014,7 +45014,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
@@ -46780,7 +46780,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="25" bestFit="1" customWidth="1"/>
@@ -51323,7 +51323,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -52603,7 +52603,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
@@ -53589,7 +53589,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="39" customWidth="1"/>
@@ -54653,9 +54653,11 @@
   <sheetPr codeName="Hoja34"/>
   <dimension ref="A1:AX17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
@@ -55673,108 +55675,125 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="17" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="29">
+    <row r="1" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
         <v>64</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31" t="s">
         <v>446</v>
       </c>
-      <c r="S1" s="91" t="s">
+      <c r="S2" s="91" t="s">
         <v>445</v>
       </c>
-      <c r="T1" s="31"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="98" t="s">
+      <c r="T2" s="31"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="98" t="s">
         <v>449</v>
       </c>
-      <c r="X1" s="98" t="s">
+      <c r="X2" s="98" t="s">
         <v>444</v>
       </c>
-      <c r="Y1" s="98"/>
-      <c r="Z1" s="170" t="s">
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="170" t="s">
         <v>450</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" s="99">
-        <v>1</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" s="137" t="s">
-        <v>389</v>
-      </c>
-      <c r="X2" s="99" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y2" s="99"/>
-      <c r="Z2" s="28" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -55784,16 +55803,12 @@
       <c r="B3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="C3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="28" t="s">
-        <v>0</v>
-      </c>
+      <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
@@ -55806,69 +55821,73 @@
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
       <c r="R3" s="96"/>
-      <c r="S3" s="28" t="s">
-        <v>146</v>
+      <c r="S3" s="30" t="s">
+        <v>0</v>
       </c>
       <c r="T3" s="28" t="s">
-        <v>349</v>
+        <v>0</v>
       </c>
       <c r="U3" s="99">
         <v>1</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="V3" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="137" t="s">
+        <v>389</v>
+      </c>
+      <c r="X3" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="96"/>
+      <c r="S4" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="T4" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="U4" s="99">
+        <v>1</v>
+      </c>
+      <c r="V4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="100"/>
-      <c r="Y3" s="101"/>
-      <c r="Z3" s="144"/>
-    </row>
-    <row r="4" spans="1:26" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="T4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="W4" s="137" t="s">
-        <v>395</v>
-      </c>
-      <c r="X4" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="132"/>
+      <c r="W4" s="100"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="144"/>
     </row>
     <row r="5" spans="1:26" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
@@ -55881,11 +55900,9 @@
         <v>0</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>16</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -55900,21 +55917,25 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="T5" s="115" t="s">
-        <v>366</v>
+        <v>0</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>0</v>
       </c>
       <c r="U5" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="V5" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="W5" s="22"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
+        <v>13</v>
+      </c>
+      <c r="V5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="137" t="s">
+        <v>395</v>
+      </c>
+      <c r="X5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="132"/>
     </row>
     <row r="6" spans="1:26" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
@@ -55927,9 +55948,11 @@
         <v>0</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -55944,111 +55967,155 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="T6" s="22" t="s">
-        <v>0</v>
+        <v>300</v>
+      </c>
+      <c r="T6" s="115" t="s">
+        <v>366</v>
       </c>
       <c r="U6" s="49" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V6" s="22" t="s">
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="W6" s="22"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="100"/>
-      <c r="B7" s="100"/>
-      <c r="C7" s="28" t="s">
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+    </row>
+    <row r="7" spans="1:26" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="V7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="100"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="102"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="99"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="28"/>
-      <c r="X7" s="99"/>
-      <c r="Y7" s="99"/>
-      <c r="Z7" s="100"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="31" t="s">
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="102"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="99"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="99"/>
+      <c r="Y8" s="99"/>
+      <c r="Z8" s="100"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="S8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="T8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="U8" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="V8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="W8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="X8" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="95"/>
-      <c r="Z8" s="31" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="X9" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="95"/>
+      <c r="Z9" s="31" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T5" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T6" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -56056,108 +56123,125 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="17" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="29">
+    <row r="1" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
         <v>64</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31" t="s">
         <v>447</v>
       </c>
-      <c r="S1" s="91" t="s">
+      <c r="S2" s="91" t="s">
         <v>448</v>
       </c>
-      <c r="T1" s="31"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="98" t="s">
+      <c r="T2" s="31"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="98" t="s">
         <v>451</v>
       </c>
-      <c r="X1" s="98" t="s">
+      <c r="X2" s="98" t="s">
         <v>444</v>
       </c>
-      <c r="Y1" s="98"/>
-      <c r="Z1" s="170" t="s">
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="170" t="s">
         <v>450</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" s="99">
-        <v>1</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" s="137" t="s">
-        <v>389</v>
-      </c>
-      <c r="X2" s="99" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y2" s="99"/>
-      <c r="Z2" s="28" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -56167,16 +56251,12 @@
       <c r="B3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="C3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="28" t="s">
-        <v>0</v>
-      </c>
+      <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
@@ -56189,70 +56269,74 @@
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
       <c r="R3" s="96"/>
-      <c r="S3" s="28" t="s">
-        <v>146</v>
+      <c r="S3" s="30" t="s">
+        <v>0</v>
       </c>
       <c r="T3" s="28" t="s">
-        <v>349</v>
+        <v>0</v>
       </c>
       <c r="U3" s="99">
         <v>1</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="V3" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="137" t="s">
+        <v>389</v>
+      </c>
+      <c r="X3" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="96"/>
+      <c r="S4" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="T4" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="U4" s="99">
+        <v>1</v>
+      </c>
+      <c r="V4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="100"/>
-      <c r="X3" s="110"/>
-      <c r="Y3" s="101"/>
-      <c r="Z3" s="144"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="T4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="W4" s="137" t="s">
-        <v>395</v>
-      </c>
-      <c r="X4" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="132"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="144"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
@@ -56265,11 +56349,9 @@
         <v>0</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>16</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -56284,21 +56366,25 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="T5" s="115" t="s">
-        <v>366</v>
+        <v>0</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>0</v>
       </c>
       <c r="U5" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="V5" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="W5" s="22"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
+        <v>13</v>
+      </c>
+      <c r="V5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="137" t="s">
+        <v>395</v>
+      </c>
+      <c r="X5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="132"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
@@ -56311,9 +56397,11 @@
         <v>0</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -56328,111 +56416,155 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="T6" s="22" t="s">
-        <v>0</v>
+        <v>300</v>
+      </c>
+      <c r="T6" s="115" t="s">
+        <v>366</v>
       </c>
       <c r="U6" s="49" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V6" s="22" t="s">
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="W6" s="22"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="100"/>
-      <c r="B7" s="100"/>
-      <c r="C7" s="28" t="s">
+      <c r="A7" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="V7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="100"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="102"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="99"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="28"/>
-      <c r="X7" s="99"/>
-      <c r="Y7" s="99"/>
-      <c r="Z7" s="100"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="31" t="s">
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="102"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="99"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="99"/>
+      <c r="Y8" s="99"/>
+      <c r="Z8" s="100"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="S8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="T8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="U8" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="V8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="W8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="X8" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="95"/>
-      <c r="Z8" s="31" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="X9" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="95"/>
+      <c r="Z9" s="31" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T5" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T6" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -56446,7 +56578,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16" width="0" hidden="1" customWidth="1"/>
@@ -56959,7 +57091,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" style="7" customWidth="1"/>
@@ -62305,7 +62437,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="10.7109375" customWidth="1"/>
@@ -65176,7 +65308,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" customWidth="1"/>
@@ -67222,7 +67354,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="10.7109375" style="2" customWidth="1"/>
@@ -68475,7 +68607,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="42" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="38" customWidth="1"/>
@@ -69228,7 +69360,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="56" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="10.7109375" style="56" customWidth="1"/>

</xml_diff>